<commit_message>
Update scripts and upload guide pictures
</commit_message>
<xml_diff>
--- a/rem_conference_deadlines.xlsx
+++ b/rem_conference_deadlines.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cesarlandin/Projects/remindr/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7C8FE78E-B55A-164F-A470-76E53A44E2BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F78E6C8-AB35-C042-83CA-C87E0D2E215A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="1000" windowWidth="25040" windowHeight="13860"/>
+    <workbookView xWindow="35580" yWindow="500" windowWidth="25040" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rem_conference_deadlines" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>deadline</t>
   </si>
@@ -77,12 +77,15 @@
   </si>
   <si>
     <t>https://usconf.uni.edu</t>
+  </si>
+  <si>
+    <t>2022_08_06</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -917,10 +920,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -954,8 +959,8 @@
       <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1">
-        <v>44779</v>
+      <c r="B2" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>